<commit_message>
updated schedules, audio and instructions
</commit_message>
<xml_diff>
--- a/conditions/schedules/train_x_first/x_decreasing_steps/bottom_left/inputTest.xlsx
+++ b/conditions/schedules/train_x_first/x_decreasing_steps/bottom_left/inputTest.xlsx
@@ -1,21 +1,95 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giancarlodeiana/Desktop/g-casa_children_task/conditions/schedules/train_x_first/x_decreasing_steps/bottom_left/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E0CAA1-7615-1D44-99C5-DD6CFBB39F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="15680" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="21">
+  <si>
+    <t>trialTrain</t>
+  </si>
+  <si>
+    <t>x_fixStart</t>
+  </si>
+  <si>
+    <t>y_fixStart</t>
+  </si>
+  <si>
+    <t>x_corrSteps</t>
+  </si>
+  <si>
+    <t>y_corrSteps</t>
+  </si>
+  <si>
+    <t>x_nrSteps</t>
+  </si>
+  <si>
+    <t>y_nrSteps</t>
+  </si>
+  <si>
+    <t>alienID</t>
+  </si>
+  <si>
+    <t>testlen</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>trial_label</t>
+  </si>
+  <si>
+    <t>test_exp</t>
+  </si>
+  <si>
+    <t>train_1D_sec_repeat</t>
+  </si>
+  <si>
+    <t>train_2D_new</t>
+  </si>
+  <si>
+    <t>untrained</t>
+  </si>
+  <si>
+    <t>train_1D_sec_new</t>
+  </si>
+  <si>
+    <t>untrained_1D_first_leftout</t>
+  </si>
+  <si>
+    <t>train_1D_first_repeat</t>
+  </si>
+  <si>
+    <t>train_2D_repeat</t>
+  </si>
+  <si>
+    <t>train_1D_first_new</t>
+  </si>
+  <si>
+    <t>untrained_1D_sec_leftout</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,17 +133,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -107,7 +189,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -141,6 +223,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -175,9 +258,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -350,71 +434,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>trialTrain</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>x_fixStart</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>y_fixStart</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>x_corrSteps</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>y_corrSteps</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>x_nrSteps</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>y_nrSteps</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>alienID</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>testlen</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>trial_label</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -434,7 +498,7 @@
         <v>3</v>
       </c>
       <c r="G2">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>31</v>
@@ -442,18 +506,14 @@
       <c r="I2">
         <v>72</v>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>train_1D_sec_repeat</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -481,18 +541,14 @@
       <c r="I3">
         <v>72</v>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>train_2D_new</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -520,18 +576,14 @@
       <c r="I4">
         <v>72</v>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -551,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>61</v>
@@ -559,18 +611,14 @@
       <c r="I5">
         <v>72</v>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>train_1D_sec_new</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
+      <c r="J5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -598,18 +646,14 @@
       <c r="I6">
         <v>72</v>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>untrained_1D_first_leftout</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
+      <c r="J6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -637,18 +681,14 @@
       <c r="I7">
         <v>72</v>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>train_1D_first_repeat</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
+      <c r="J7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -676,18 +716,14 @@
       <c r="I8">
         <v>72</v>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
+      <c r="J8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -715,18 +751,14 @@
       <c r="I9">
         <v>72</v>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
+      <c r="J9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -754,18 +786,14 @@
       <c r="I10">
         <v>72</v>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
+      <c r="J10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -793,18 +821,14 @@
       <c r="I11">
         <v>72</v>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>train_2D_repeat</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
+      <c r="J11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -832,18 +856,14 @@
       <c r="I12">
         <v>72</v>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
+      <c r="J12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -871,18 +891,14 @@
       <c r="I13">
         <v>72</v>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>train_2D_new</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
+      <c r="J13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -910,18 +926,14 @@
       <c r="I14">
         <v>72</v>
       </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>train_1D_first_new</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
+      <c r="J14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -941,7 +953,7 @@
         <v>5</v>
       </c>
       <c r="G15">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H15">
         <v>11</v>
@@ -949,18 +961,14 @@
       <c r="I15">
         <v>72</v>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>train_1D_sec_new</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
+      <c r="J15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -988,18 +996,14 @@
       <c r="I16">
         <v>72</v>
       </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
+      <c r="J16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1027,18 +1031,14 @@
       <c r="I17">
         <v>72</v>
       </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
+      <c r="J17" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1066,18 +1066,14 @@
       <c r="I18">
         <v>72</v>
       </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
+      <c r="J18" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1105,18 +1101,14 @@
       <c r="I19">
         <v>72</v>
       </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
+      <c r="J19" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1136,7 +1128,7 @@
         <v>4</v>
       </c>
       <c r="G20">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H20">
         <v>21</v>
@@ -1144,18 +1136,14 @@
       <c r="I20">
         <v>72</v>
       </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>train_1D_sec_new</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
+      <c r="J20" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1175,7 +1163,7 @@
         <v>2</v>
       </c>
       <c r="G21">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H21">
         <v>41</v>
@@ -1183,18 +1171,14 @@
       <c r="I21">
         <v>72</v>
       </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>train_1D_sec_repeat</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
+      <c r="J21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1222,18 +1206,14 @@
       <c r="I22">
         <v>72</v>
       </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
+      <c r="J22" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1261,18 +1241,14 @@
       <c r="I23">
         <v>72</v>
       </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>train_1D_first_repeat</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
+      <c r="J23" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1300,18 +1276,14 @@
       <c r="I24">
         <v>72</v>
       </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
+      <c r="J24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1331,7 +1303,7 @@
         <v>1</v>
       </c>
       <c r="G25">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H25">
         <v>51</v>
@@ -1339,18 +1311,14 @@
       <c r="I25">
         <v>72</v>
       </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>untrained_1D_sec_leftout</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
+      <c r="J25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1378,18 +1346,14 @@
       <c r="I26">
         <v>72</v>
       </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
+      <c r="J26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1417,18 +1381,14 @@
       <c r="I27">
         <v>72</v>
       </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>train_2D_repeat</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
+      <c r="J27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1456,18 +1416,14 @@
       <c r="I28">
         <v>72</v>
       </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
+      <c r="J28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1495,18 +1451,14 @@
       <c r="I29">
         <v>72</v>
       </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
+      <c r="J29" t="s">
+        <v>11</v>
+      </c>
+      <c r="K29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1534,18 +1486,14 @@
       <c r="I30">
         <v>72</v>
       </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>train_2D_new</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
+      <c r="J30" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1573,18 +1521,14 @@
       <c r="I31">
         <v>72</v>
       </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
+      <c r="J31" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1612,18 +1556,14 @@
       <c r="I32">
         <v>72</v>
       </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
+      <c r="J32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1651,18 +1591,14 @@
       <c r="I33">
         <v>72</v>
       </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
+      <c r="J33" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1690,18 +1626,14 @@
       <c r="I34">
         <v>72</v>
       </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
+      <c r="J34" t="s">
+        <v>11</v>
+      </c>
+      <c r="K34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1729,18 +1661,14 @@
       <c r="I35">
         <v>72</v>
       </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
+      <c r="J35" t="s">
+        <v>11</v>
+      </c>
+      <c r="K35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1768,18 +1696,14 @@
       <c r="I36">
         <v>72</v>
       </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>train_1D_first_new</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
+      <c r="J36" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1807,18 +1731,14 @@
       <c r="I37">
         <v>72</v>
       </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
+      <c r="J37" t="s">
+        <v>11</v>
+      </c>
+      <c r="K37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1846,18 +1766,14 @@
       <c r="I38">
         <v>72</v>
       </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
+      <c r="J38" t="s">
+        <v>11</v>
+      </c>
+      <c r="K38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1877,7 +1793,7 @@
         <v>3</v>
       </c>
       <c r="G39">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H39">
         <v>31</v>
@@ -1885,18 +1801,14 @@
       <c r="I39">
         <v>72</v>
       </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>train_1D_sec_new</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
+      <c r="J39" t="s">
+        <v>11</v>
+      </c>
+      <c r="K39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1924,18 +1836,14 @@
       <c r="I40">
         <v>72</v>
       </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
+      <c r="J40" t="s">
+        <v>11</v>
+      </c>
+      <c r="K40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1963,18 +1871,14 @@
       <c r="I41">
         <v>72</v>
       </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>train_2D_repeat</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
+      <c r="J41" t="s">
+        <v>11</v>
+      </c>
+      <c r="K41" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2002,18 +1906,14 @@
       <c r="I42">
         <v>72</v>
       </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
+      <c r="J42" t="s">
+        <v>11</v>
+      </c>
+      <c r="K42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2041,18 +1941,14 @@
       <c r="I43">
         <v>72</v>
       </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
+      <c r="J43" t="s">
+        <v>11</v>
+      </c>
+      <c r="K43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2080,18 +1976,14 @@
       <c r="I44">
         <v>72</v>
       </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>untrained_1D_first_leftout</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
+      <c r="J44" t="s">
+        <v>11</v>
+      </c>
+      <c r="K44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2119,18 +2011,14 @@
       <c r="I45">
         <v>72</v>
       </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
+      <c r="J45" t="s">
+        <v>11</v>
+      </c>
+      <c r="K45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2158,18 +2046,14 @@
       <c r="I46">
         <v>72</v>
       </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>train_1D_first_repeat</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
+      <c r="J46" t="s">
+        <v>11</v>
+      </c>
+      <c r="K46" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2197,18 +2081,14 @@
       <c r="I47">
         <v>72</v>
       </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>train_2D_new</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
+      <c r="J47" t="s">
+        <v>11</v>
+      </c>
+      <c r="K47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2236,18 +2116,14 @@
       <c r="I48">
         <v>72</v>
       </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
+      <c r="J48" t="s">
+        <v>11</v>
+      </c>
+      <c r="K48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2275,18 +2151,14 @@
       <c r="I49">
         <v>72</v>
       </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
+      <c r="J49" t="s">
+        <v>11</v>
+      </c>
+      <c r="K49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2314,18 +2186,14 @@
       <c r="I50">
         <v>72</v>
       </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
+      <c r="J50" t="s">
+        <v>11</v>
+      </c>
+      <c r="K50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2345,7 +2213,7 @@
         <v>4</v>
       </c>
       <c r="G51">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H51">
         <v>21</v>
@@ -2353,18 +2221,14 @@
       <c r="I51">
         <v>72</v>
       </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>train_1D_sec_repeat</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
+      <c r="J51" t="s">
+        <v>11</v>
+      </c>
+      <c r="K51" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2384,7 +2248,7 @@
         <v>2</v>
       </c>
       <c r="G52">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H52">
         <v>41</v>
@@ -2392,18 +2256,14 @@
       <c r="I52">
         <v>72</v>
       </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>train_1D_sec_new</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
+      <c r="J52" t="s">
+        <v>11</v>
+      </c>
+      <c r="K52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2431,18 +2291,14 @@
       <c r="I53">
         <v>72</v>
       </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
+      <c r="J53" t="s">
+        <v>11</v>
+      </c>
+      <c r="K53" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2470,18 +2326,14 @@
       <c r="I54">
         <v>72</v>
       </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
+      <c r="J54" t="s">
+        <v>11</v>
+      </c>
+      <c r="K54" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2509,18 +2361,14 @@
       <c r="I55">
         <v>72</v>
       </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
+      <c r="J55" t="s">
+        <v>11</v>
+      </c>
+      <c r="K55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2548,18 +2396,14 @@
       <c r="I56">
         <v>72</v>
       </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>train_2D_new</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
+      <c r="J56" t="s">
+        <v>11</v>
+      </c>
+      <c r="K56" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2579,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="G57">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H57">
         <v>61</v>
@@ -2587,18 +2431,14 @@
       <c r="I57">
         <v>72</v>
       </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>train_1D_sec_repeat</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
+      <c r="J57" t="s">
+        <v>11</v>
+      </c>
+      <c r="K57" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2626,18 +2466,14 @@
       <c r="I58">
         <v>72</v>
       </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
+      <c r="J58" t="s">
+        <v>11</v>
+      </c>
+      <c r="K58" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2665,18 +2501,14 @@
       <c r="I59">
         <v>72</v>
       </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>train_1D_first_new</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
+      <c r="J59" t="s">
+        <v>11</v>
+      </c>
+      <c r="K59" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2704,18 +2536,14 @@
       <c r="I60">
         <v>72</v>
       </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
+      <c r="J60" t="s">
+        <v>11</v>
+      </c>
+      <c r="K60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2743,18 +2571,14 @@
       <c r="I61">
         <v>72</v>
       </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
+      <c r="J61" t="s">
+        <v>11</v>
+      </c>
+      <c r="K61" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2782,18 +2606,14 @@
       <c r="I62">
         <v>72</v>
       </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
+      <c r="J62" t="s">
+        <v>11</v>
+      </c>
+      <c r="K62" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2821,18 +2641,14 @@
       <c r="I63">
         <v>72</v>
       </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>train_2D_repeat</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
+      <c r="J63" t="s">
+        <v>11</v>
+      </c>
+      <c r="K63" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2860,18 +2676,14 @@
       <c r="I64">
         <v>72</v>
       </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>train_1D_first_new</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
+      <c r="J64" t="s">
+        <v>11</v>
+      </c>
+      <c r="K64" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2899,18 +2711,14 @@
       <c r="I65">
         <v>72</v>
       </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>train_1D_first_repeat</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
+      <c r="J65" t="s">
+        <v>11</v>
+      </c>
+      <c r="K65" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2930,7 +2738,7 @@
         <v>1</v>
       </c>
       <c r="G66">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H66">
         <v>51</v>
@@ -2938,18 +2746,14 @@
       <c r="I66">
         <v>72</v>
       </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>untrained_1D_sec_leftout</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
+      <c r="J66" t="s">
+        <v>11</v>
+      </c>
+      <c r="K66" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2977,18 +2781,14 @@
       <c r="I67">
         <v>72</v>
       </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
+      <c r="J67" t="s">
+        <v>11</v>
+      </c>
+      <c r="K67" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3016,18 +2816,14 @@
       <c r="I68">
         <v>72</v>
       </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
+      <c r="J68" t="s">
+        <v>11</v>
+      </c>
+      <c r="K68" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3055,18 +2851,14 @@
       <c r="I69">
         <v>72</v>
       </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
+      <c r="J69" t="s">
+        <v>11</v>
+      </c>
+      <c r="K69" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3094,18 +2886,14 @@
       <c r="I70">
         <v>72</v>
       </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>train_2D_repeat</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
+      <c r="J70" t="s">
+        <v>11</v>
+      </c>
+      <c r="K70" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3133,18 +2921,14 @@
       <c r="I71">
         <v>72</v>
       </c>
-      <c r="J71" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
+      <c r="J71" t="s">
+        <v>11</v>
+      </c>
+      <c r="K71" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3172,18 +2956,14 @@
       <c r="I72">
         <v>72</v>
       </c>
-      <c r="J72" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>untrained</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
+      <c r="J72" t="s">
+        <v>11</v>
+      </c>
+      <c r="K72" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3203,7 +2983,7 @@
         <v>5</v>
       </c>
       <c r="G73">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H73">
         <v>11</v>
@@ -3211,15 +2991,11 @@
       <c r="I73">
         <v>72</v>
       </c>
-      <c r="J73" t="inlineStr">
-        <is>
-          <t>test_exp</t>
-        </is>
-      </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>train_1D_sec_repeat</t>
-        </is>
+      <c r="J73" t="s">
+        <v>11</v>
+      </c>
+      <c r="K73" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>